<commit_message>
fix in labels evaluation
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_labels.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_labels.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1447,59 +1447,47 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9021078431372549</v>
+        <v>0.8775025799793603</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8372549019607842</v>
+        <v>0.9183006535947712</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8673351158645277</v>
+        <v>0.8970424205718324</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8674019607843138</v>
+        <v>0.878809769521844</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8366013071895424</v>
+        <v>0.9300653594771241</v>
       </c>
       <c r="G17" t="n">
-        <v>0.8512554112554112</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.8450796107916851</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.8019607843137255</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.8209886887306241</v>
-      </c>
+        <v>0.903428975193681</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
-        <v>0.8862745098039216</v>
+        <v>0.8669762641898865</v>
       </c>
       <c r="L17" t="n">
-        <v>0.8143790849673203</v>
+        <v>0.9065359477124183</v>
       </c>
       <c r="M17" t="n">
-        <v>0.8476381461675579</v>
+        <v>0.8859313094607213</v>
       </c>
       <c r="N17" t="n">
-        <v>0.8796078431372549</v>
+        <v>0.8795846233230135</v>
       </c>
       <c r="O17" t="n">
-        <v>0.8379084967320261</v>
+        <v>0.9183006535947712</v>
       </c>
       <c r="P17" t="n">
-        <v>0.8565667175961293</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.8700773993808049</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.9183006535947713</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0.8924351877912249</v>
-      </c>
+        <v>0.8972849090496149</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1508,59 +1496,47 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.7226613965744401</v>
+        <v>0.9421826625386996</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8384210526315791</v>
+        <v>0.8078947368421051</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7760193295077016</v>
+        <v>0.8692109692109693</v>
       </c>
       <c r="E18" t="n">
-        <v>0.757519292301901</v>
+        <v>0.9546826625386997</v>
       </c>
       <c r="F18" t="n">
-        <v>0.848421052631579</v>
+        <v>0.8078947368421051</v>
       </c>
       <c r="G18" t="n">
-        <v>0.8003100775193799</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.7414492753623187</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.7973684210526316</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.7666007595016163</v>
-      </c>
+        <v>0.873972873972874</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
-        <v>0.7209169960474309</v>
+        <v>0.9311532507739937</v>
       </c>
       <c r="L18" t="n">
-        <v>0.848421052631579</v>
+        <v>0.7978947368421052</v>
       </c>
       <c r="M18" t="n">
-        <v>0.7785147152589014</v>
+        <v>0.8587004587004585</v>
       </c>
       <c r="N18" t="n">
-        <v>0.7554616977225672</v>
+        <v>0.9311532507739937</v>
       </c>
       <c r="O18" t="n">
-        <v>0.858421052631579</v>
+        <v>0.7978947368421052</v>
       </c>
       <c r="P18" t="n">
-        <v>0.8026412410303504</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0.8473684210526315</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0.8378947368421054</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0.8423076923076923</v>
-      </c>
+        <v>0.8587004587004585</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1569,59 +1545,47 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8441957344341245</v>
+        <v>0.7925077211118401</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8315789473684211</v>
+        <v>0.9263157894736842</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8331324626061468</v>
+        <v>0.8520716425209365</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8340476190476191</v>
+        <v>0.799064935064935</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8315789473684211</v>
+        <v>0.9368421052631579</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8308801108801109</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.7288655185394315</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.7473684210526316</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.72969667503984</v>
-      </c>
+        <v>0.8610469545580154</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
-        <v>0.786118387975973</v>
+        <v>0.7386363636363636</v>
       </c>
       <c r="L19" t="n">
-        <v>0.8</v>
+        <v>0.9368421052631579</v>
       </c>
       <c r="M19" t="n">
-        <v>0.7886012328117591</v>
+        <v>0.8251547510419492</v>
       </c>
       <c r="N19" t="n">
-        <v>0.8234210526315791</v>
+        <v>0.7534914361001317</v>
       </c>
       <c r="O19" t="n">
-        <v>0.8736842105263157</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="P19" t="n">
-        <v>0.8457889393017911</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0.7689619305179946</v>
-      </c>
-      <c r="R19" t="n">
-        <v>0.873684210526316</v>
-      </c>
-      <c r="S19" t="n">
-        <v>0.8171281863194571</v>
-      </c>
+        <v>0.8384437875867997</v>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1630,59 +1594,47 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.7487787723785166</v>
+        <v>0.825701754385965</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7977941176470589</v>
+        <v>0.7485294117647059</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7672381606205135</v>
+        <v>0.781008921248076</v>
       </c>
       <c r="E20" t="n">
-        <v>0.7136114796795912</v>
+        <v>0.8380392156862746</v>
       </c>
       <c r="F20" t="n">
-        <v>0.75</v>
+        <v>0.7838235294117647</v>
       </c>
       <c r="G20" t="n">
-        <v>0.7281657708128296</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.7596078431372549</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.7029411764705882</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.7232576692703958</v>
-      </c>
+        <v>0.8094028520499108</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
-        <v>0.7605042016806722</v>
+        <v>0.8564102564102564</v>
       </c>
       <c r="L20" t="n">
-        <v>0.726470588235294</v>
+        <v>0.6294117647058822</v>
       </c>
       <c r="M20" t="n">
-        <v>0.7368391541446571</v>
+        <v>0.7201566555431961</v>
       </c>
       <c r="N20" t="n">
-        <v>0.8043128654970761</v>
+        <v>0.8597435897435897</v>
       </c>
       <c r="O20" t="n">
-        <v>0.7860294117647058</v>
+        <v>0.6529411764705881</v>
       </c>
       <c r="P20" t="n">
-        <v>0.7921721963467694</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0.7538461538461538</v>
-      </c>
-      <c r="R20" t="n">
-        <v>0.7014705882352942</v>
-      </c>
-      <c r="S20" t="n">
-        <v>0.7234803921568627</v>
-      </c>
+        <v>0.7385474601408972</v>
+      </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1691,363 +1643,656 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9414181286549708</v>
+        <v>0.8347924158221641</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7861904761904761</v>
+        <v>0.8342857142857143</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8545379387484651</v>
+        <v>0.8332294062526622</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9200421396628826</v>
+        <v>0.8609394698868382</v>
       </c>
       <c r="F21" t="n">
-        <v>0.7852380952380953</v>
+        <v>0.8438095238095238</v>
       </c>
       <c r="G21" t="n">
-        <v>0.8460517197359303</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.7562101836782145</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.7261904761904763</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.7377895398458433</v>
-      </c>
+        <v>0.8513013105651253</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
-        <v>0.9287988241548613</v>
+        <v>0.8088104153664795</v>
       </c>
       <c r="L21" t="n">
-        <v>0.8157142857142856</v>
+        <v>0.8538095238095238</v>
       </c>
       <c r="M21" t="n">
-        <v>0.862679776363987</v>
+        <v>0.8287315010570824</v>
       </c>
       <c r="N21" t="n">
-        <v>0.9335130718954249</v>
+        <v>0.823794466403162</v>
       </c>
       <c r="O21" t="n">
-        <v>0.7947619047619048</v>
+        <v>0.8633333333333333</v>
       </c>
       <c r="P21" t="n">
-        <v>0.8564817449027975</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0.826155462184874</v>
-      </c>
-      <c r="R21" t="n">
-        <v>0.7266666666666668</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0.7713472235936935</v>
-      </c>
+        <v>0.8421883693919995</v>
+      </c>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Ensemble_F</t>
+          <t>RF_F</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.8775025799793603</v>
+        <v>0.8856372549019607</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9183006535947712</v>
+        <v>0.8026143790849674</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8970424205718324</v>
+        <v>0.8412433155080216</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8883006535947711</v>
+        <v>0.8617927170868347</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9183006535947712</v>
+        <v>0.7797385620915032</v>
       </c>
       <c r="G22" t="n">
-        <v>0.902084437378555</v>
+        <v>0.8169117647058822</v>
       </c>
       <c r="H22" t="n">
-        <v>0.8146395400265369</v>
+        <v>0.8375101214574899</v>
       </c>
       <c r="I22" t="n">
-        <v>0.7660130718954248</v>
+        <v>0.8124183006535948</v>
       </c>
       <c r="J22" t="n">
-        <v>0.7873942253448896</v>
+        <v>0.8207655502392344</v>
       </c>
       <c r="K22" t="n">
-        <v>0.8669762641898865</v>
+        <v>0.8714705882352941</v>
       </c>
       <c r="L22" t="n">
+        <v>0.7908496732026145</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.8283645276292335</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.8766666666666666</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.8143790849673203</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.8430194805194805</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.8700316968892819</v>
+      </c>
+      <c r="R22" t="n">
         <v>0.9065359477124183</v>
       </c>
-      <c r="M22" t="n">
-        <v>0.8859313094607213</v>
-      </c>
-      <c r="N22" t="n">
-        <v>0.8346491228070176</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0.9294117647058823</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0.8777041671778514</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0.837218045112782</v>
-      </c>
-      <c r="R22" t="n">
-        <v>0.8137254901960784</v>
-      </c>
       <c r="S22" t="n">
-        <v>0.8222183888218044</v>
+        <v>0.886539604186663</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Ensemble_NF</t>
+          <t>RF_NF</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9421826625386996</v>
+        <v>0.7099472990777338</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8078947368421051</v>
+        <v>0.8384210526315791</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8692109692109693</v>
+        <v>0.768448605657908</v>
       </c>
       <c r="E23" t="n">
-        <v>0.943888888888889</v>
+        <v>0.7424987864919215</v>
       </c>
       <c r="F23" t="n">
-        <v>0.8178947368421052</v>
+        <v>0.8278947368421055</v>
       </c>
       <c r="G23" t="n">
-        <v>0.8748203842940685</v>
+        <v>0.7813279743512301</v>
       </c>
       <c r="H23" t="n">
-        <v>0.784628091969053</v>
+        <v>0.7742181540808544</v>
       </c>
       <c r="I23" t="n">
+        <v>0.8173684210526316</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.7911215915867078</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.7301739130434782</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.8384210526315791</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.7791754756871037</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.7081501831501831</v>
+      </c>
+      <c r="O23" t="n">
         <v>0.848421052631579</v>
       </c>
-      <c r="J23" t="n">
-        <v>0.8137692596020207</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.9311532507739937</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0.7978947368421052</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0.8587004587004585</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0.9307189542483659</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0.758421052631579</v>
-      </c>
       <c r="P23" t="n">
-        <v>0.8336846355422207</v>
+        <v>0.7709426754162753</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.8099054114399383</v>
+        <v>0.8454720133667502</v>
       </c>
       <c r="R23" t="n">
-        <v>0.8084210526315788</v>
+        <v>0.8278947368421052</v>
       </c>
       <c r="S23" t="n">
-        <v>0.8059700999367237</v>
+        <v>0.8360156018564234</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Ensemble_PM</t>
+          <t>RF_PM</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.7925077211118401</v>
+        <v>0.8541197579510271</v>
       </c>
       <c r="C24" t="n">
-        <v>0.9263157894736842</v>
+        <v>0.8315789473684211</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8520716425209365</v>
+        <v>0.8402062065733439</v>
       </c>
       <c r="E24" t="n">
-        <v>0.8119138755980861</v>
+        <v>0.8480247678018575</v>
       </c>
       <c r="F24" t="n">
-        <v>0.8842105263157893</v>
+        <v>0.8736842105263157</v>
       </c>
       <c r="G24" t="n">
-        <v>0.8447665041568972</v>
+        <v>0.857203615098352</v>
       </c>
       <c r="H24" t="n">
-        <v>0.7987581699346404</v>
+        <v>0.7741993888464477</v>
       </c>
       <c r="I24" t="n">
-        <v>0.7578947368421052</v>
+        <v>0.8105263157894737</v>
       </c>
       <c r="J24" t="n">
-        <v>0.7770616770616771</v>
+        <v>0.7866198571076619</v>
       </c>
       <c r="K24" t="n">
-        <v>0.7386363636363636</v>
+        <v>0.8303581480439066</v>
       </c>
       <c r="L24" t="n">
-        <v>0.9368421052631579</v>
+        <v>0.8105263157894737</v>
       </c>
       <c r="M24" t="n">
-        <v>0.8251547510419492</v>
+        <v>0.8179338590378386</v>
       </c>
       <c r="N24" t="n">
-        <v>0.785972360972361</v>
+        <v>0.8050597508263412</v>
       </c>
       <c r="O24" t="n">
-        <v>0.9473684210526315</v>
+        <v>0.8210526315789475</v>
       </c>
       <c r="P24" t="n">
-        <v>0.8579636982416335</v>
+        <v>0.8112578744157692</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.8066666666666669</v>
+        <v>0.7748917748917749</v>
       </c>
       <c r="R24" t="n">
-        <v>0.8315789473684211</v>
+        <v>0.8736842105263157</v>
       </c>
       <c r="S24" t="n">
-        <v>0.8185724185724187</v>
+        <v>0.821219512195122</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Ensemble_M</t>
+          <t>RF_M</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.825701754385965</v>
+        <v>0.7616410912190965</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7485294117647059</v>
+        <v>0.8102941176470588</v>
       </c>
       <c r="D25" t="n">
-        <v>0.781008921248076</v>
+        <v>0.7793885102708632</v>
       </c>
       <c r="E25" t="n">
-        <v>0.7983900928792569</v>
+        <v>0.7439164086687307</v>
       </c>
       <c r="F25" t="n">
-        <v>0.7970588235294118</v>
+        <v>0.7624999999999998</v>
       </c>
       <c r="G25" t="n">
-        <v>0.7949042950513538</v>
+        <v>0.751029836176895</v>
       </c>
       <c r="H25" t="n">
-        <v>0.7881715506715508</v>
+        <v>0.7496031746031747</v>
       </c>
       <c r="I25" t="n">
-        <v>0.7375</v>
+        <v>0.6786764705882352</v>
       </c>
       <c r="J25" t="n">
-        <v>0.7585752688172043</v>
+        <v>0.7088569394791996</v>
       </c>
       <c r="K25" t="n">
-        <v>0.8564102564102564</v>
+        <v>0.731552250190694</v>
       </c>
       <c r="L25" t="n">
-        <v>0.6294117647058822</v>
+        <v>0.7977941176470589</v>
       </c>
       <c r="M25" t="n">
-        <v>0.7201566555431961</v>
+        <v>0.7579477204477205</v>
       </c>
       <c r="N25" t="n">
-        <v>0.910989010989011</v>
+        <v>0.7645704948646126</v>
       </c>
       <c r="O25" t="n">
-        <v>0.7139705882352941</v>
+        <v>0.7625</v>
       </c>
       <c r="P25" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.7598665429025961</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.8004481792717086</v>
+        <v>0.7678991596638656</v>
       </c>
       <c r="R25" t="n">
-        <v>0.725735294117647</v>
+        <v>0.7727941176470587</v>
       </c>
       <c r="S25" t="n">
-        <v>0.7592583807716635</v>
+        <v>0.7668180785827845</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
+          <t>RF_V</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9298331613347093</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.7947619047619047</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.8559604138551506</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9041083099906629</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.8147619047619047</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.8555017938843354</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.7802756892230577</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.7557142857142857</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.7670933431138824</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.9111111111111111</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.7842857142857144</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.840944669365722</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.9075421396628827</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.7547619047619047</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.8222915222915222</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.8629411764705882</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.7271428571428571</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0.7875486012328119</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble_F</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.8775025799793603</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.9183006535947712</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.8970424205718324</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.8883006535947711</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.9183006535947712</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.902084437378555</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.8192676767676769</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.8124183006535948</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.8125757575757575</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.8669762641898865</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.9065359477124183</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.8859313094607213</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.8346491228070176</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.9294117647058823</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.8777041671778514</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.8572222222222223</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.8477124183006535</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.8514430014430016</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble_NF</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.9421826625386996</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.8078947368421051</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.8692109692109693</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.943888888888889</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.8178947368421052</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.8748203842940685</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.7932900432900433</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.8263157894736842</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.8075261324041814</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.9311532507739937</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.7978947368421052</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.8587004587004585</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.9307189542483659</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.758421052631579</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.8336846355422207</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.8142395762132605</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.7978947368421052</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.8029768605378361</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble_PM</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.7925077211118401</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.9263157894736842</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.8520716425209365</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.8119138755980861</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.8842105263157893</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.8447665041568972</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.7786354775828459</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.8526315789473685</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.809889674924</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.7386363636363636</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.9368421052631579</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.8251547510419492</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.785972360972361</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.8579636982416335</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.8157302346776032</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.8631578947368421</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0.8380948619202793</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble_M</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.825701754385965</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.7485294117647059</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.781008921248076</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.7983900928792569</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.7970588235294118</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.7949042950513538</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.8066793681035167</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.6904411764705882</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.7344887955182072</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.8564102564102564</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.6294117647058822</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.7201566555431961</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.910989010989011</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.7139705882352941</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.8200962436256554</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.7132352941176471</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.7587602783048704</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
           <t>Ensemble_V</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B31" t="n">
         <v>0.8347924158221641</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C31" t="n">
         <v>0.8342857142857143</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D31" t="n">
         <v>0.8332294062526622</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E31" t="n">
         <v>0.8639553429027114</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F31" t="n">
         <v>0.8638095238095238</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G31" t="n">
         <v>0.8628499955329223</v>
       </c>
-      <c r="H26" t="n">
-        <v>0.7332248110394565</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.7747619047619047</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.7522155364015829</v>
-      </c>
-      <c r="K26" t="n">
+      <c r="H31" t="n">
+        <v>0.7757787050747071</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.7452380952380953</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.7579824010056568</v>
+      </c>
+      <c r="K31" t="n">
         <v>0.8088104153664795</v>
       </c>
-      <c r="L26" t="n">
+      <c r="L31" t="n">
         <v>0.8538095238095238</v>
       </c>
-      <c r="M26" t="n">
+      <c r="M31" t="n">
         <v>0.8287315010570824</v>
       </c>
-      <c r="N26" t="n">
+      <c r="N31" t="n">
         <v>0.8558095238095238</v>
       </c>
-      <c r="O26" t="n">
+      <c r="O31" t="n">
         <v>0.9023809523809524</v>
       </c>
-      <c r="P26" t="n">
+      <c r="P31" t="n">
         <v>0.8776215724890168</v>
       </c>
-      <c r="Q26" t="n">
-        <v>0.7773122529644269</v>
-      </c>
-      <c r="R26" t="n">
-        <v>0.8147619047619049</v>
-      </c>
-      <c r="S26" t="n">
-        <v>0.7948854397634885</v>
+      <c r="Q31" t="n">
+        <v>0.8062280701754385</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.8442857142857143</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.8219733924611974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>